<commit_message>
finalizacion cambio id config multivendor
</commit_message>
<xml_diff>
--- a/src/test/resources/datafiles/Cambio_config_robot_Multivendor_ConPagos.xlsx
+++ b/src/test/resources/datafiles/Cambio_config_robot_Multivendor_ConPagos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cfroc\Documents\trabajo 2021\grupo HDI\Trabajo Bancolombia\Framework SBDD\autoStarc\HDISerenityStarc\src\test\resources\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC38BA1-3779-41AD-B6A3-94B717112335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D257480-0AC3-47A4-A97E-D0A450B7F70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1202,8 +1202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="G125" sqref="G125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1235,7 +1235,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>203</v>
+        <v>274</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>273</v>
@@ -1347,7 +1347,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>273</v>
@@ -1361,7 +1361,7 @@
         <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>273</v>
@@ -1375,7 +1375,7 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>273</v>
@@ -1389,7 +1389,7 @@
         <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>273</v>
@@ -1403,7 +1403,7 @@
         <v>26</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>273</v>
@@ -1417,7 +1417,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>273</v>
@@ -1431,7 +1431,7 @@
         <v>30</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D16" s="5" t="s">
         <v>273</v>
@@ -1445,7 +1445,7 @@
         <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>273</v>
@@ -1459,7 +1459,7 @@
         <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>273</v>
@@ -1473,7 +1473,7 @@
         <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>273</v>
@@ -1487,7 +1487,7 @@
         <v>38</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>273</v>
@@ -1501,7 +1501,7 @@
         <v>40</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>273</v>
@@ -1515,7 +1515,7 @@
         <v>42</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>273</v>
@@ -1529,7 +1529,7 @@
         <v>44</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>273</v>
@@ -1543,7 +1543,7 @@
         <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>273</v>
@@ -1557,7 +1557,7 @@
         <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>273</v>
@@ -1571,7 +1571,7 @@
         <v>50</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>273</v>
@@ -1585,7 +1585,7 @@
         <v>52</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>273</v>
@@ -1599,7 +1599,7 @@
         <v>54</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D28" s="5" t="s">
         <v>273</v>
@@ -1613,7 +1613,7 @@
         <v>56</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D29" s="5" t="s">
         <v>273</v>
@@ -1627,7 +1627,7 @@
         <v>58</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>273</v>
@@ -1641,7 +1641,7 @@
         <v>60</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>273</v>
@@ -1655,7 +1655,7 @@
         <v>62</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>273</v>
@@ -1669,7 +1669,7 @@
         <v>64</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>273</v>
@@ -1683,7 +1683,7 @@
         <v>66</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>273</v>
@@ -1697,7 +1697,7 @@
         <v>68</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>273</v>
@@ -1711,7 +1711,7 @@
         <v>70</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>273</v>
@@ -1725,7 +1725,7 @@
         <v>72</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>273</v>
@@ -1739,7 +1739,7 @@
         <v>74</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>273</v>
@@ -1753,7 +1753,7 @@
         <v>76</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>273</v>
@@ -1767,7 +1767,7 @@
         <v>78</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>273</v>
@@ -1781,7 +1781,7 @@
         <v>80</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D41" s="5" t="s">
         <v>273</v>
@@ -1795,7 +1795,7 @@
         <v>82</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D42" s="5" t="s">
         <v>273</v>
@@ -1809,7 +1809,7 @@
         <v>84</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D43" s="5" t="s">
         <v>273</v>
@@ -1823,7 +1823,7 @@
         <v>86</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>273</v>
@@ -1837,7 +1837,7 @@
         <v>88</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>273</v>
@@ -1851,7 +1851,7 @@
         <v>90</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D46" s="5" t="s">
         <v>273</v>
@@ -1865,7 +1865,7 @@
         <v>92</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>273</v>
@@ -1879,7 +1879,7 @@
         <v>94</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>273</v>
@@ -1893,7 +1893,7 @@
         <v>96</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>273</v>
@@ -1907,7 +1907,7 @@
         <v>98</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>273</v>
@@ -1921,7 +1921,7 @@
         <v>100</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D51" s="5" t="s">
         <v>273</v>
@@ -1935,7 +1935,7 @@
         <v>102</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>273</v>
@@ -1949,7 +1949,7 @@
         <v>104</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>273</v>
@@ -1963,7 +1963,7 @@
         <v>106</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>273</v>
@@ -1977,7 +1977,7 @@
         <v>108</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>273</v>
@@ -1991,7 +1991,7 @@
         <v>110</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>273</v>
@@ -2005,7 +2005,7 @@
         <v>112</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>273</v>
@@ -2019,7 +2019,7 @@
         <v>114</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>273</v>
@@ -2033,7 +2033,7 @@
         <v>116</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>273</v>
@@ -2047,7 +2047,7 @@
         <v>118</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>273</v>
@@ -2061,7 +2061,7 @@
         <v>120</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>273</v>
@@ -2075,7 +2075,7 @@
         <v>122</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>273</v>
@@ -2089,7 +2089,7 @@
         <v>124</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>273</v>
@@ -2103,7 +2103,7 @@
         <v>126</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>273</v>
@@ -2117,7 +2117,7 @@
         <v>128</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>273</v>
@@ -2131,7 +2131,7 @@
         <v>130</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>273</v>
@@ -2145,7 +2145,7 @@
         <v>132</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>273</v>
@@ -2159,7 +2159,7 @@
         <v>134</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>273</v>
@@ -2173,7 +2173,7 @@
         <v>136</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>273</v>
@@ -2187,7 +2187,7 @@
         <v>138</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>273</v>
@@ -2201,7 +2201,7 @@
         <v>140</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>273</v>
@@ -2215,7 +2215,7 @@
         <v>142</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>273</v>
@@ -2229,7 +2229,7 @@
         <v>144</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>273</v>
@@ -2243,7 +2243,7 @@
         <v>146</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>273</v>
@@ -2257,7 +2257,7 @@
         <v>148</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>273</v>
@@ -2271,7 +2271,7 @@
         <v>150</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>273</v>
@@ -2285,7 +2285,7 @@
         <v>152</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>273</v>
@@ -2299,7 +2299,7 @@
         <v>154</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>273</v>
@@ -2313,7 +2313,7 @@
         <v>156</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>273</v>
@@ -2327,7 +2327,7 @@
         <v>158</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>273</v>
@@ -2341,7 +2341,7 @@
         <v>160</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>273</v>
@@ -2355,7 +2355,7 @@
         <v>162</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>273</v>
@@ -2369,7 +2369,7 @@
         <v>164</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>273</v>
@@ -2383,7 +2383,7 @@
         <v>166</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>273</v>
@@ -2397,7 +2397,7 @@
         <v>168</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>273</v>
@@ -2411,7 +2411,7 @@
         <v>170</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>273</v>
@@ -2425,7 +2425,7 @@
         <v>172</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>273</v>
@@ -2439,7 +2439,7 @@
         <v>174</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>273</v>
@@ -2453,7 +2453,7 @@
         <v>176</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>273</v>
@@ -2467,7 +2467,7 @@
         <v>178</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>273</v>
@@ -2481,7 +2481,7 @@
         <v>180</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D91" s="5" t="s">
         <v>273</v>
@@ -2495,7 +2495,7 @@
         <v>182</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>273</v>
@@ -2509,7 +2509,7 @@
         <v>184</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>273</v>
@@ -2523,7 +2523,7 @@
         <v>186</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>273</v>
@@ -2537,7 +2537,7 @@
         <v>188</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>273</v>
@@ -2551,7 +2551,7 @@
         <v>190</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>273</v>
@@ -2565,7 +2565,7 @@
         <v>192</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>273</v>
@@ -2579,7 +2579,7 @@
         <v>194</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>273</v>
@@ -2593,7 +2593,7 @@
         <v>196</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>273</v>
@@ -2607,7 +2607,7 @@
         <v>198</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>273</v>
@@ -2621,7 +2621,7 @@
         <v>200</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>273</v>
@@ -2635,7 +2635,7 @@
         <v>202</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>273</v>
@@ -2649,7 +2649,7 @@
         <v>205</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>273</v>
@@ -2663,7 +2663,7 @@
         <v>207</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>273</v>
@@ -2677,7 +2677,7 @@
         <v>209</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>273</v>
@@ -2691,7 +2691,7 @@
         <v>211</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>273</v>
@@ -2705,7 +2705,7 @@
         <v>213</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>273</v>
@@ -2719,7 +2719,7 @@
         <v>215</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>273</v>
@@ -2733,7 +2733,7 @@
         <v>217</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>273</v>
@@ -2747,7 +2747,7 @@
         <v>219</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>273</v>
@@ -2761,7 +2761,7 @@
         <v>221</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>273</v>
@@ -2775,7 +2775,7 @@
         <v>223</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>273</v>
@@ -2789,7 +2789,7 @@
         <v>225</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>273</v>
@@ -2803,7 +2803,7 @@
         <v>227</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>273</v>
@@ -2817,7 +2817,7 @@
         <v>229</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>273</v>
@@ -2831,7 +2831,7 @@
         <v>231</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>273</v>
@@ -2845,7 +2845,7 @@
         <v>233</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>273</v>
@@ -2859,7 +2859,7 @@
         <v>235</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>273</v>
@@ -2873,7 +2873,7 @@
         <v>237</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>273</v>
@@ -2887,7 +2887,7 @@
         <v>239</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>273</v>
@@ -2901,7 +2901,7 @@
         <v>241</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>273</v>
@@ -2915,7 +2915,7 @@
         <v>243</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>273</v>
@@ -2929,7 +2929,7 @@
         <v>245</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>273</v>
@@ -2943,7 +2943,7 @@
         <v>247</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>273</v>
@@ -2957,7 +2957,7 @@
         <v>249</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>273</v>
@@ -2971,7 +2971,7 @@
         <v>251</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>273</v>
@@ -2985,7 +2985,7 @@
         <v>253</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D127" s="5" t="s">
         <v>273</v>
@@ -2999,7 +2999,7 @@
         <v>255</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D128" s="5" t="s">
         <v>273</v>
@@ -3013,7 +3013,7 @@
         <v>257</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D129" s="5" t="s">
         <v>273</v>
@@ -3027,7 +3027,7 @@
         <v>259</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D130" s="5" t="s">
         <v>273</v>
@@ -3041,7 +3041,7 @@
         <v>261</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D131" s="5" t="s">
         <v>273</v>
@@ -3055,7 +3055,7 @@
         <v>263</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D132" s="5" t="s">
         <v>273</v>
@@ -3069,7 +3069,7 @@
         <v>265</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D133" s="5" t="s">
         <v>273</v>
@@ -3083,7 +3083,7 @@
         <v>266</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D134" s="5" t="s">
         <v>273</v>
@@ -3097,7 +3097,7 @@
         <v>267</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>274</v>
+        <v>203</v>
       </c>
       <c r="D135" s="5" t="s">
         <v>273</v>

</xml_diff>